<commit_message>
All englisch in naming excel
</commit_message>
<xml_diff>
--- a/Naming.xlsx
+++ b/Naming.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="265">
   <si>
     <t>A</t>
   </si>
@@ -536,9 +536,6 @@
     <t>Global</t>
   </si>
   <si>
-    <t>Eindeutigkeit</t>
-  </si>
-  <si>
     <t>billTo</t>
   </si>
   <si>
@@ -816,6 +813,9 @@
   </si>
   <si>
     <t>Number, code, user name, … for the dependent resource</t>
+  </si>
+  <si>
+    <t>Uniqueness</t>
   </si>
 </sst>
 </file>
@@ -1840,6 +1840,24 @@
   <dxfs count="5">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1878,24 +1896,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1910,7 +1910,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:D50" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:D50" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:D50"/>
   <sortState ref="A2:D46">
     <sortCondition ref="A1:A46"/>
@@ -2191,7 +2191,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2205,10 +2207,10 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Q3" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z3" s="73" t="s">
         <v>241</v>
-      </c>
-      <c r="Z3" s="73" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2217,7 +2219,7 @@
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -2292,13 +2294,13 @@
         <v>24</v>
       </c>
       <c r="AA5" s="95" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" s="112" t="s">
         <v>0</v>
@@ -2341,12 +2343,12 @@
       </c>
       <c r="X6" s="108"/>
       <c r="Y6" s="109" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Z6" s="110"/>
       <c r="AA6" s="96"/>
       <c r="AC6" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
@@ -2380,12 +2382,12 @@
         <v>0</v>
       </c>
       <c r="AD7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="2:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="94" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="6"/>
@@ -2416,12 +2418,12 @@
         <v>1</v>
       </c>
       <c r="AD8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C9" s="67"/>
       <c r="D9" s="6"/>
@@ -2452,7 +2454,7 @@
         <v>2</v>
       </c>
       <c r="AD9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
@@ -2460,64 +2462,64 @@
         <v>148</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F10" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="H10" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="H10" s="61" t="s">
-        <v>225</v>
-      </c>
       <c r="I10" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L10" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O10" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R10" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T10" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U10" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W10" s="90"/>
       <c r="X10" s="91"/>
@@ -2531,7 +2533,7 @@
         <v>3</v>
       </c>
       <c r="AD10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
@@ -2539,64 +2541,64 @@
         <v>154</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F11" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="H11" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="H11" s="61" t="s">
-        <v>225</v>
-      </c>
       <c r="I11" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K11" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L11" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="M11" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="N11" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="N11" s="31" t="s">
+      <c r="O11" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q11" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="O11" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q11" s="28" t="s">
-        <v>231</v>
-      </c>
       <c r="R11" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T11" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U11" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W11" s="90"/>
       <c r="X11" s="91"/>
@@ -2610,7 +2612,7 @@
         <v>146</v>
       </c>
       <c r="AD11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
@@ -2618,64 +2620,64 @@
         <v>156</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G12" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="H12" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="H12" s="61" t="s">
-        <v>225</v>
-      </c>
       <c r="I12" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K12" s="80" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L12" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="N12" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="O12" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q12" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="N12" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O12" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q12" s="28" t="s">
-        <v>231</v>
-      </c>
       <c r="R12" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U12" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W12" s="90"/>
       <c r="X12" s="91"/>
@@ -2689,7 +2691,7 @@
         <v>147</v>
       </c>
       <c r="AD12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
@@ -2697,64 +2699,64 @@
         <v>12</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F13" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G13" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="H13" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="H13" s="61" t="s">
-        <v>225</v>
-      </c>
       <c r="I13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K13" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L13" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="L13" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>228</v>
-      </c>
       <c r="N13" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O13" s="55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R13" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U13" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V13" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W13" s="90"/>
       <c r="X13" s="91"/>
@@ -2768,7 +2770,7 @@
         <v>155</v>
       </c>
       <c r="AD13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
@@ -2776,64 +2778,64 @@
         <v>10</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H14" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K14" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L14" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F14" s="64" t="s">
+      <c r="N14" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="O14" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="G14" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H14" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J14" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K14" s="80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L14" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="N14" s="31" t="s">
+      <c r="P14" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q14" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="O14" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q14" s="28" t="s">
-        <v>231</v>
-      </c>
       <c r="R14" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U14" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W14" s="90"/>
       <c r="X14" s="91"/>
@@ -2847,70 +2849,70 @@
         <v>150</v>
       </c>
       <c r="AD14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="45"/>
       <c r="C15" s="67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F15" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H15" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K15" s="80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L15" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N15" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O15" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R15" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T15" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U15" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W15" s="90"/>
       <c r="X15" s="91"/>
@@ -2923,67 +2925,67 @@
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H16" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K16" s="80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L16" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N16" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O16" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q16" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R16" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U16" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W16" s="90"/>
       <c r="X16" s="91"/>
@@ -2999,64 +3001,64 @@
         <v>148</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K17" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F17" s="64" t="s">
-        <v>223</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H17" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J17" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K17" s="80" t="s">
-        <v>235</v>
-      </c>
       <c r="L17" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N17" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O17" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q17" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R17" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T17" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U17" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W17" s="90"/>
       <c r="X17" s="91"/>
@@ -3067,7 +3069,7 @@
         <v>tvd20abat</v>
       </c>
       <c r="AC17" s="75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
@@ -3075,64 +3077,64 @@
         <v>154</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K18" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="E18" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F18" s="64" t="s">
+      <c r="L18" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="N18" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="O18" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="G18" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J18" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K18" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="L18" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="N18" s="31" t="s">
+      <c r="P18" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q18" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="O18" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q18" s="28" t="s">
-        <v>231</v>
-      </c>
       <c r="R18" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U18" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V18" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W18" s="90"/>
       <c r="X18" s="91"/>
@@ -3152,64 +3154,64 @@
         <v>156</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F19" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K19" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="E19" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F19" s="64" t="s">
+      <c r="L19" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="N19" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="O19" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="G19" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H19" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K19" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="L19" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="M19" s="8" t="s">
+      <c r="P19" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q19" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="N19" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O19" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P19" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q19" s="28" t="s">
-        <v>231</v>
-      </c>
       <c r="R19" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U19" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V19" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W19" s="90"/>
       <c r="X19" s="91"/>
@@ -3223,7 +3225,7 @@
         <v>90</v>
       </c>
       <c r="AE19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
@@ -3231,64 +3233,64 @@
         <v>12</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F20" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H20" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K20" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="E20" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F20" s="64" t="s">
+      <c r="L20" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N20" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="O20" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="G20" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H20" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K20" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="L20" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N20" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="O20" s="55" t="s">
-        <v>224</v>
-      </c>
       <c r="P20" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R20" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U20" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W20" s="90"/>
       <c r="X20" s="91"/>
@@ -3302,70 +3304,70 @@
         <v>20</v>
       </c>
       <c r="AE20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B21" s="45"/>
       <c r="C21" s="67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H21" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K21" s="80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L21" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O21" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q21" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R21" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U21" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W21" s="90"/>
       <c r="X21" s="91"/>
@@ -3379,70 +3381,70 @@
         <v>10</v>
       </c>
       <c r="AE21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B22" s="45"/>
       <c r="C22" s="67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F22" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H22" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K22" s="80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L22" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O22" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R22" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T22" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U22" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V22" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W22" s="90"/>
       <c r="X22" s="91"/>
@@ -3456,72 +3458,72 @@
         <v>50</v>
       </c>
       <c r="AE22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="94" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" s="67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F23" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H23" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K23" s="80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L23" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N23" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O23" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R23" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T23" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U23" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V23" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W23" s="90"/>
       <c r="X23" s="91"/>
@@ -3537,64 +3539,64 @@
         <v>160</v>
       </c>
       <c r="C24" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F24" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H24" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K24" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L24" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N24" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="O24" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q24" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="R24" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="S24" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F24" s="64" t="s">
-        <v>223</v>
-      </c>
-      <c r="G24" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H24" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J24" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K24" s="80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L24" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N24" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="O24" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P24" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q24" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R24" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>236</v>
-      </c>
       <c r="T24" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U24" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W24" s="90"/>
       <c r="X24" s="91"/>
@@ -3614,75 +3616,75 @@
         <v>161</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F25" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G25" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="H25" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="H25" s="61" t="s">
-        <v>225</v>
-      </c>
       <c r="I25" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K25" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N25" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="O25" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q25" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="R25" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="J25" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K25" s="80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L25" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N25" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="O25" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P25" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q25" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R25" s="52" t="s">
-        <v>234</v>
-      </c>
-      <c r="S25" s="10" t="s">
-        <v>222</v>
-      </c>
       <c r="T25" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U25" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V25" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W25" s="90"/>
       <c r="X25" s="91"/>
       <c r="Y25" s="85"/>
       <c r="Z25" s="11"/>
       <c r="AA25" s="98" t="str">
-        <f t="shared" ref="AA25:AA30" si="1">_xlfn.CONCAT(F25:V25)</f>
-        <v>20abapsrv001vhd</v>
+        <f t="shared" ref="AA25:AA28" si="1">_xlfn.CONCAT(C25:V25)</f>
+        <v>tvd20abapsrv001vhd</v>
       </c>
       <c r="AD25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AE25" t="s">
         <v>167</v>
@@ -3690,67 +3692,67 @@
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B26" s="45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C26" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F26" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K26" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L26" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N26" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="O26" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q26" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="R26" s="52" t="s">
+        <v>231</v>
+      </c>
+      <c r="S26" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E26" s="40" t="s">
+      <c r="T26" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="F26" s="64" t="s">
-        <v>223</v>
-      </c>
-      <c r="G26" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H26" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K26" s="80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L26" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N26" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="O26" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P26" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q26" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R26" s="52" t="s">
-        <v>232</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>238</v>
-      </c>
       <c r="U26" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V26" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W26" s="90"/>
       <c r="X26" s="91"/>
@@ -3758,7 +3760,7 @@
       <c r="Z26" s="11"/>
       <c r="AA26" s="98" t="str">
         <f t="shared" si="1"/>
-        <v>20abapsrv001nic</v>
+        <v>tvd20abapsrv001nic</v>
       </c>
       <c r="AD26" s="74" t="s">
         <v>168</v>
@@ -3772,64 +3774,64 @@
         <v>162</v>
       </c>
       <c r="C27" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K27" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L27" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N27" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="O27" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="R27" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="S27" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F27" s="64" t="s">
+      <c r="T27" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="U27" s="49" t="s">
         <v>223</v>
       </c>
-      <c r="G27" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H27" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J27" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K27" s="80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L27" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N27" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="O27" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P27" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q27" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R27" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="S27" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="T27" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="U27" s="49" t="s">
-        <v>224</v>
-      </c>
       <c r="V27" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="W27" s="90"/>
       <c r="X27" s="91"/>
@@ -3837,13 +3839,13 @@
       <c r="Z27" s="11"/>
       <c r="AA27" s="98" t="str">
         <f t="shared" si="1"/>
-        <v>20abapsrv001pip01</v>
+        <v>tvd20abapsrv001pip01</v>
       </c>
       <c r="AD27" s="99" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AE27" s="100" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.25">
@@ -3851,64 +3853,64 @@
         <v>163</v>
       </c>
       <c r="C28" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F28" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="K28" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="L28" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N28" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="O28" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q28" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="R28" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="S28" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F28" s="64" t="s">
+      <c r="T28" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="U28" s="49" t="s">
         <v>223</v>
       </c>
-      <c r="G28" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="H28" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="K28" s="80" t="s">
-        <v>227</v>
-      </c>
-      <c r="L28" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N28" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="O28" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="P28" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q28" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="R28" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="S28" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="T28" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="U28" s="49" t="s">
-        <v>224</v>
-      </c>
       <c r="V28" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W28" s="90"/>
       <c r="X28" s="91"/>
@@ -3916,7 +3918,7 @@
       <c r="Z28" s="11"/>
       <c r="AA28" s="98" t="str">
         <f t="shared" si="1"/>
-        <v>20abapsrv001pip02</v>
+        <v>tvd20abapsrv001pip02</v>
       </c>
     </row>
     <row r="29" spans="2:31" x14ac:dyDescent="0.25">
@@ -3946,7 +3948,7 @@
       <c r="Y29" s="85"/>
       <c r="Z29" s="11"/>
       <c r="AA29" s="98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AA25:AA30" si="2">_xlfn.CONCAT(F29:V29)</f>
         <v/>
       </c>
       <c r="AD29" s="105" t="s">
@@ -3981,14 +3983,14 @@
       <c r="Y30" s="86"/>
       <c r="Z30" s="17"/>
       <c r="AA30" s="96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="AD30" t="s">
         <v>149</v>
       </c>
       <c r="AE30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
@@ -4001,7 +4003,7 @@
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>171</v>
+        <v>264</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -4031,12 +4033,12 @@
         <v>148</v>
       </c>
       <c r="C34" s="82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B36" s="77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -4446,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -4629,57 +4631,57 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" t="s">
         <v>212</v>
-      </c>
-      <c r="B47" t="s">
-        <v>214</v>
-      </c>
-      <c r="C47" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" t="s">
         <v>215</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>216</v>
-      </c>
-      <c r="C48" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" t="s">
         <v>218</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>219</v>
-      </c>
-      <c r="C49" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" t="s">
         <v>239</v>
-      </c>
-      <c r="B50" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:C47 B49:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C47">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:C48">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:C48">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4706,119 +4708,119 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" t="s">
         <v>199</v>
-      </c>
-      <c r="C3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" t="s">
         <v>176</v>
       </c>
-      <c r="C4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>177</v>
-      </c>
-      <c r="E4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" t="s">
         <v>179</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>180</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>181</v>
-      </c>
-      <c r="E5" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
         <v>183</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>184</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>185</v>
-      </c>
-      <c r="E6" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" t="s">
         <v>187</v>
-      </c>
-      <c r="C7" t="s">
-        <v>188</v>
       </c>
       <c r="D7" s="76">
         <v>3.4</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" t="s">
         <v>190</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>191</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>192</v>
-      </c>
-      <c r="E8" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" t="s">
         <v>194</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>195</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>196</v>
-      </c>
-      <c r="E9" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -4826,7 +4828,7 @@
         <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OMS and cert update
</commit_message>
<xml_diff>
--- a/Naming.xlsx
+++ b/Naming.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="266">
   <si>
     <t>A</t>
   </si>
@@ -95,33 +95,18 @@
     <t>gwlo</t>
   </si>
   <si>
-    <t xml:space="preserve">local gateway </t>
-  </si>
-  <si>
     <t>vipi</t>
   </si>
   <si>
-    <t>virtual public ip</t>
-  </si>
-  <si>
     <t>vipn</t>
   </si>
   <si>
-    <t>virtual Private Network</t>
-  </si>
-  <si>
     <t>gatw</t>
   </si>
   <si>
-    <t>gateway (object)</t>
-  </si>
-  <si>
     <t>rgat</t>
   </si>
   <si>
-    <t>remote network gateway (Object/Subnet)</t>
-  </si>
-  <si>
     <t>vilb</t>
   </si>
   <si>
@@ -263,9 +248,6 @@
     <t>gatc</t>
   </si>
   <si>
-    <t>gateway connection</t>
-  </si>
-  <si>
     <t>(gateway (object))</t>
   </si>
   <si>
@@ -287,15 +269,9 @@
     <t>runb</t>
   </si>
   <si>
-    <t>Automation runbook</t>
-  </si>
-  <si>
     <t>webh</t>
   </si>
   <si>
-    <t>Runbook webhook</t>
-  </si>
-  <si>
     <t>apsp</t>
   </si>
   <si>
@@ -311,9 +287,6 @@
     <t>vmsc</t>
   </si>
   <si>
-    <t>virtual machine scale set</t>
-  </si>
-  <si>
     <t>agat</t>
   </si>
   <si>
@@ -816,6 +789,36 @@
   </si>
   <si>
     <t>Uniqueness</t>
+  </si>
+  <si>
+    <t>schj</t>
+  </si>
+  <si>
+    <t>Virtual Private Network</t>
+  </si>
+  <si>
+    <t>Virtual public ip</t>
+  </si>
+  <si>
+    <t>Virtual machine scale set</t>
+  </si>
+  <si>
+    <t>Remote network gateway (Object/Subnet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local gateway </t>
+  </si>
+  <si>
+    <t>Gateway connection</t>
+  </si>
+  <si>
+    <t>Gateway (object)</t>
+  </si>
+  <si>
+    <t>Runbook</t>
+  </si>
+  <si>
+    <t>Webhook</t>
   </si>
 </sst>
 </file>
@@ -1910,9 +1913,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:D50" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D50"/>
-  <sortState ref="A2:D46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:D51" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D51"/>
+  <sortState ref="A2:D51">
     <sortCondition ref="A1:A46"/>
   </sortState>
   <tableColumns count="4">
@@ -2191,9 +2194,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2207,10 +2208,10 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Q3" s="73" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="Z3" s="73" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2219,7 +2220,7 @@
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -2231,22 +2232,22 @@
         <v>3</v>
       </c>
       <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4">
         <v>5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>6</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>7</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>8</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>9</v>
-      </c>
-      <c r="K5" s="4">
-        <v>4</v>
       </c>
       <c r="L5" s="4">
         <v>10</v>
@@ -2294,13 +2295,13 @@
         <v>24</v>
       </c>
       <c r="AA5" s="95" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="42" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C6" s="112" t="s">
         <v>0</v>
@@ -2320,35 +2321,35 @@
         <v>3</v>
       </c>
       <c r="L6" s="120" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="M6" s="121"/>
       <c r="N6" s="122"/>
       <c r="O6" s="123" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="P6" s="124"/>
       <c r="Q6" s="125"/>
       <c r="R6" s="126" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="S6" s="127"/>
       <c r="T6" s="128"/>
       <c r="U6" s="111" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="V6" s="110"/>
       <c r="W6" s="107" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="X6" s="108"/>
       <c r="Y6" s="109" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="Z6" s="110"/>
       <c r="AA6" s="96"/>
       <c r="AC6" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
@@ -2382,12 +2383,12 @@
         <v>0</v>
       </c>
       <c r="AD7" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="2:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="94" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="6"/>
@@ -2418,12 +2419,12 @@
         <v>1</v>
       </c>
       <c r="AD8" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="44" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C9" s="67"/>
       <c r="D9" s="6"/>
@@ -2454,72 +2455,72 @@
         <v>2</v>
       </c>
       <c r="AD9" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H10" s="61" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="L10" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O10" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R10" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T10" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U10" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W10" s="90"/>
       <c r="X10" s="91"/>
@@ -2533,72 +2534,72 @@
         <v>3</v>
       </c>
       <c r="AD10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="45" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F11" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H11" s="61" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I11" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K11" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L11" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="N11" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="J11" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K11" s="80" t="s">
-        <v>226</v>
-      </c>
-      <c r="L11" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N11" s="31" t="s">
-        <v>229</v>
-      </c>
       <c r="O11" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R11" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T11" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U11" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W11" s="90"/>
       <c r="X11" s="91"/>
@@ -2609,75 +2610,75 @@
         <v>tvd20abaprsg001</v>
       </c>
       <c r="AC11" s="69" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="AD11" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="45" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F12" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="H12" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K12" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L12" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="M12" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="N12" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="H12" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J12" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K12" s="80" t="s">
-        <v>226</v>
-      </c>
-      <c r="L12" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="N12" s="31" t="s">
-        <v>232</v>
-      </c>
       <c r="O12" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R12" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U12" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W12" s="90"/>
       <c r="X12" s="91"/>
@@ -2688,10 +2689,10 @@
         <v>tvd20abapngw001</v>
       </c>
       <c r="AC12" s="69" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AD12" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
@@ -2699,64 +2700,64 @@
         <v>12</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F13" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H13" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K13" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L13" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N13" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K13" s="80" t="s">
-        <v>226</v>
-      </c>
-      <c r="L13" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N13" s="31" t="s">
-        <v>233</v>
-      </c>
       <c r="O13" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R13" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U13" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V13" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W13" s="90"/>
       <c r="X13" s="91"/>
@@ -2767,10 +2768,10 @@
         <v>tvd20abapsrv001</v>
       </c>
       <c r="AC13" s="69" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD13" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
@@ -2778,64 +2779,64 @@
         <v>10</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H14" s="61" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I14" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K14" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L14" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="N14" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="J14" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K14" s="80" t="s">
-        <v>226</v>
-      </c>
-      <c r="L14" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="N14" s="31" t="s">
-        <v>229</v>
-      </c>
       <c r="O14" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R14" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U14" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W14" s="90"/>
       <c r="X14" s="91"/>
@@ -2846,73 +2847,73 @@
         <v>tvd20abapstg001</v>
       </c>
       <c r="AC14" s="69" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="AD14" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="45"/>
       <c r="C15" s="67" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F15" s="64" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H15" s="61" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="K15" s="80" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="L15" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N15" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O15" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R15" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T15" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U15" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W15" s="90"/>
       <c r="X15" s="91"/>
@@ -2925,67 +2926,67 @@
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="44" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H16" s="61" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="K16" s="80" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="L16" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N16" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O16" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q16" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R16" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U16" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W16" s="90"/>
       <c r="X16" s="91"/>
@@ -2998,67 +2999,67 @@
     </row>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F17" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H17" s="61" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="K17" s="80" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="L17" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N17" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O17" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q17" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R17" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T17" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U17" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W17" s="90"/>
       <c r="X17" s="91"/>
@@ -3069,72 +3070,72 @@
         <v>tvd20abat</v>
       </c>
       <c r="AC17" s="75" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B18" s="45" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F18" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H18" s="61" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I18" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K18" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="L18" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="N18" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="J18" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K18" s="80" t="s">
-        <v>234</v>
-      </c>
-      <c r="L18" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="N18" s="31" t="s">
-        <v>229</v>
-      </c>
       <c r="O18" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R18" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T18" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U18" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V18" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W18" s="90"/>
       <c r="X18" s="91"/>
@@ -3151,67 +3152,67 @@
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B19" s="45" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F19" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K19" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="L19" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="M19" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="N19" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="H19" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K19" s="80" t="s">
-        <v>234</v>
-      </c>
-      <c r="L19" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="N19" s="31" t="s">
-        <v>232</v>
-      </c>
       <c r="O19" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q19" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R19" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U19" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V19" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W19" s="90"/>
       <c r="X19" s="91"/>
@@ -3225,7 +3226,7 @@
         <v>90</v>
       </c>
       <c r="AE19" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
@@ -3233,64 +3234,64 @@
         <v>12</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F20" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H20" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K20" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="L20" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N20" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K20" s="80" t="s">
-        <v>234</v>
-      </c>
-      <c r="L20" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N20" s="31" t="s">
-        <v>233</v>
-      </c>
       <c r="O20" s="55" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R20" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U20" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W20" s="90"/>
       <c r="X20" s="91"/>
@@ -3304,70 +3305,70 @@
         <v>20</v>
       </c>
       <c r="AE20" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B21" s="45"/>
       <c r="C21" s="67" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H21" s="61" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="K21" s="80" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="L21" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O21" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q21" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R21" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U21" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W21" s="90"/>
       <c r="X21" s="91"/>
@@ -3381,70 +3382,70 @@
         <v>10</v>
       </c>
       <c r="AE21" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B22" s="45"/>
       <c r="C22" s="67" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F22" s="64" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H22" s="61" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="K22" s="80" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="L22" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O22" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R22" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T22" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U22" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V22" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W22" s="90"/>
       <c r="X22" s="91"/>
@@ -3458,72 +3459,72 @@
         <v>50</v>
       </c>
       <c r="AE22" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="94" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C23" s="67" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F23" s="64" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H23" s="61" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="K23" s="80" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="L23" s="58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N23" s="31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="O23" s="55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="R23" s="52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="T23" s="25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U23" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V23" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W23" s="90"/>
       <c r="X23" s="91"/>
@@ -3536,67 +3537,67 @@
     </row>
     <row r="24" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B24" s="45" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F24" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H24" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K24" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L24" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N24" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J24" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K24" s="80" t="s">
+      <c r="O24" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q24" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="R24" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="S24" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="L24" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N24" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O24" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="P24" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q24" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R24" s="52" t="s">
-        <v>226</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>235</v>
-      </c>
       <c r="T24" s="25" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="U24" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W24" s="90"/>
       <c r="X24" s="91"/>
@@ -3613,67 +3614,67 @@
     </row>
     <row r="25" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B25" s="45" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F25" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H25" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K25" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N25" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J25" s="34" t="s">
+      <c r="O25" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q25" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="R25" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="K25" s="80" t="s">
-        <v>226</v>
-      </c>
-      <c r="L25" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M25" s="8" t="s">
+      <c r="S25" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="T25" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="N25" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O25" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="P25" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q25" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R25" s="52" t="s">
-        <v>233</v>
-      </c>
-      <c r="S25" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>236</v>
-      </c>
       <c r="U25" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V25" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W25" s="90"/>
       <c r="X25" s="91"/>
@@ -3684,75 +3685,75 @@
         <v>tvd20abapsrv001vhd</v>
       </c>
       <c r="AD25" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="AE25" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B26" s="45" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C26" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F26" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K26" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L26" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N26" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="O26" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q26" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="R26" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="G26" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="H26" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K26" s="80" t="s">
+      <c r="S26" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="L26" s="58" t="s">
+      <c r="T26" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="M26" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N26" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O26" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="P26" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q26" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R26" s="52" t="s">
-        <v>231</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>237</v>
-      </c>
       <c r="U26" s="49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="V26" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="W26" s="90"/>
       <c r="X26" s="91"/>
@@ -3763,75 +3764,75 @@
         <v>tvd20abapsrv001nic</v>
       </c>
       <c r="AD26" s="74" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AE26" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B27" s="45" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E27" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F27" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H27" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K27" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L27" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N27" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J27" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K27" s="80" t="s">
+      <c r="O27" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="R27" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="S27" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="L27" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N27" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O27" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="P27" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q27" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R27" s="52" t="s">
-        <v>226</v>
-      </c>
-      <c r="S27" s="10" t="s">
-        <v>235</v>
-      </c>
       <c r="T27" s="25" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="U27" s="49" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="V27" s="11" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="W27" s="90"/>
       <c r="X27" s="91"/>
@@ -3842,75 +3843,75 @@
         <v>tvd20abapsrv001pip01</v>
       </c>
       <c r="AD27" s="99" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="AE27" s="100" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B28" s="45" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F28" s="64" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H28" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="K28" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="L28" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N28" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="K28" s="80" t="s">
+      <c r="O28" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q28" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="R28" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="S28" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="L28" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N28" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="O28" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="P28" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q28" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R28" s="52" t="s">
-        <v>226</v>
-      </c>
-      <c r="S28" s="10" t="s">
-        <v>235</v>
-      </c>
       <c r="T28" s="25" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="U28" s="49" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="V28" s="11" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="W28" s="90"/>
       <c r="X28" s="91"/>
@@ -3948,7 +3949,7 @@
       <c r="Y29" s="85"/>
       <c r="Z29" s="11"/>
       <c r="AA29" s="98" t="str">
-        <f t="shared" ref="AA25:AA30" si="2">_xlfn.CONCAT(F29:V29)</f>
+        <f t="shared" ref="AA29:AA30" si="2">_xlfn.CONCAT(F29:V29)</f>
         <v/>
       </c>
       <c r="AD29" s="105" t="s">
@@ -3987,31 +3988,31 @@
         <v/>
       </c>
       <c r="AD30" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="AE30" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
       <c r="AD31" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="AE31" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="AD32" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="AE32" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="2:31" x14ac:dyDescent="0.25">
@@ -4019,26 +4020,26 @@
         <v>10</v>
       </c>
       <c r="C33" s="82" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="AD33" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="AE33" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B34" s="69" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C34" s="82" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B36" s="77" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4083,10 +4084,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -4094,60 +4095,60 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4155,7 +4156,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -4163,13 +4164,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4177,7 +4178,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -4185,489 +4186,492 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>263</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" t="s">
-        <v>70</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>261</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>159</v>
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>260</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>264</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>229</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>70</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>259</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>213</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>212</v>
+        <v>58</v>
+      </c>
+      <c r="D47" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>214</v>
+        <v>257</v>
       </c>
       <c r="B48" t="s">
-        <v>215</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="B49" t="s">
-        <v>218</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>219</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="B50" t="s">
-        <v>239</v>
+        <v>131</v>
+      </c>
+      <c r="C50" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4708,127 +4712,127 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D7" s="76">
         <v>3.4</v>
       </c>
       <c r="E7" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>